<commit_message>
Add profile and client WS
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/04_Utils/04_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/04_Utils/04_LibFormula.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -147,10 +147,10 @@
     <t>Utils</t>
   </si>
   <si>
-    <t>IsLastOfMonth</t>
-  </si>
-  <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>isLastOfMonth</t>
   </si>
 </sst>
 </file>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -783,11 +783,11 @@
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -834,9 +834,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,25 +957,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -994,9 +987,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New Formula to create VM source table
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/04_Utils/04_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/04_Utils/04_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Action</t>
   </si>
@@ -161,11 +161,14 @@
   <si>
     <t>updateWorkflowStatus</t>
   </si>
+  <si>
+    <t>createTableforVM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -747,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -832,6 +835,23 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -886,6 +906,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -999,12 +1025,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
@@ -1014,6 +1034,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1027,19 +1062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>